<commit_message>
kilsys also kill the new process COMOLM and also the VISION tela "que" show the new application queue
</commit_message>
<xml_diff>
--- a/Millennium_Important_Documentation/MILL_DATA_STRUCTURES_igs_V2_2020(DRAFT).xlsx
+++ b/Millennium_Important_Documentation/MILL_DATA_STRUCTURES_igs_V2_2020(DRAFT).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\105864\Documents\Millennium\Millennium_Important_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525E15F6-1319-4F26-A960-FA7CB9993F33}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D2249A8-6AEA-4E9E-B652-FDED2ED75C54}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="35880" yWindow="1530" windowWidth="21600" windowHeight="11265" firstSheet="18" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QUEUE" sheetId="1" r:id="rId1"/>
@@ -7488,9 +7488,6 @@
     </r>
   </si>
   <si>
-    <t>Serial number from Olimpo (YYMMDD-MM-NNNNNNNNNN-CCC)</t>
-  </si>
-  <si>
     <t>MESSID=53</t>
   </si>
   <si>
@@ -7522,6 +7519,9 @@
   </si>
   <si>
     <t>SEROLM=13</t>
+  </si>
+  <si>
+    <t>Serial number from Olimpo "Transaction Serial" (YYMMDD-MM-NNNNNNNNNN-CCC)</t>
   </si>
 </sst>
 </file>
@@ -10705,14 +10705,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:O834"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J115" sqref="J115"/>
+    <sheetView showGridLines="0" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="56.453125" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="1" max="1" width="73.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
     <col min="5" max="5" width="1.453125" customWidth="1"/>
@@ -12424,7 +12424,7 @@
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>2343</v>
+        <v>2354</v>
       </c>
       <c r="B115" s="2">
         <v>113</v>
@@ -12433,7 +12433,7 @@
         <v>49</v>
       </c>
       <c r="D115" s="66" t="s">
-        <v>2354</v>
+        <v>2353</v>
       </c>
       <c r="F115" s="29">
         <v>49</v>
@@ -12605,7 +12605,7 @@
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
       <c r="B124" s="2">
         <v>122</v>
@@ -12614,7 +12614,7 @@
         <v>58</v>
       </c>
       <c r="D124" s="65" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="F124" s="30">
         <v>58</v>
@@ -12628,7 +12628,7 @@
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>2352</v>
+        <v>2351</v>
       </c>
       <c r="B125" s="2">
         <v>123</v>
@@ -12637,7 +12637,7 @@
         <v>59</v>
       </c>
       <c r="D125" s="63" t="s">
-        <v>2353</v>
+        <v>2352</v>
       </c>
       <c r="F125" s="30">
         <v>59</v>
@@ -13595,7 +13595,7 @@
         <v>105</v>
       </c>
       <c r="D171" s="66" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="F171" s="29">
         <v>105</v>
@@ -14095,7 +14095,7 @@
         <v>33</v>
       </c>
       <c r="L195" t="s">
-        <v>2347</v>
+        <v>2346</v>
       </c>
       <c r="M195">
         <v>1</v>
@@ -14120,7 +14120,7 @@
       <c r="J196" s="8"/>
       <c r="K196" s="517"/>
       <c r="L196" t="s">
-        <v>2348</v>
+        <v>2347</v>
       </c>
       <c r="M196">
         <v>2</v>
@@ -14145,7 +14145,7 @@
       <c r="J197" s="8"/>
       <c r="K197" s="517"/>
       <c r="L197" t="s">
-        <v>2349</v>
+        <v>2348</v>
       </c>
       <c r="M197">
         <v>3</v>
@@ -14170,7 +14170,7 @@
       <c r="J198" s="9"/>
       <c r="K198" s="517"/>
       <c r="L198" t="s">
-        <v>2349</v>
+        <v>2348</v>
       </c>
       <c r="M198">
         <v>4</v>
@@ -14199,7 +14199,7 @@
         <v>34</v>
       </c>
       <c r="L199" t="s">
-        <v>2350</v>
+        <v>2349</v>
       </c>
       <c r="M199">
         <v>5</v>
@@ -14224,7 +14224,7 @@
       <c r="J200" s="4"/>
       <c r="K200" s="517"/>
       <c r="L200" t="s">
-        <v>2350</v>
+        <v>2349</v>
       </c>
       <c r="M200">
         <v>6</v>
@@ -14249,7 +14249,7 @@
       <c r="J201" s="4"/>
       <c r="K201" s="517"/>
       <c r="L201" t="s">
-        <v>2350</v>
+        <v>2349</v>
       </c>
       <c r="M201">
         <v>7</v>
@@ -14274,7 +14274,7 @@
       <c r="J202" s="5"/>
       <c r="K202" s="517"/>
       <c r="L202" t="s">
-        <v>2351</v>
+        <v>2350</v>
       </c>
       <c r="M202">
         <v>8</v>
@@ -14303,7 +14303,7 @@
         <v>35</v>
       </c>
       <c r="L203" s="364" t="s">
-        <v>2351</v>
+        <v>2350</v>
       </c>
       <c r="M203">
         <v>9</v>
@@ -49362,8 +49362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="B1:AB86"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:J86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>